<commit_message>
Proyecto Fin de Carrera
Añadida tabla de inversiones 01 y 02
</commit_message>
<xml_diff>
--- a/Matriz de Requisitos.xlsx
+++ b/Matriz de Requisitos.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos 01" sheetId="1" r:id="rId1"/>
     <sheet name="Matriz de Cobertura 01" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabla de Inversion 01" sheetId="3" r:id="rId3"/>
+    <sheet name="Tabla de Inversion 02" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Matriz de Cobertura 01'!$A$1:$J$1</definedName>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -319,6 +321,99 @@
   </si>
   <si>
     <t>Los tablones de anuncios digitales solo informaran de los anuncios de los respectivos centros en los que este o de alguna notificación general.</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Coste</t>
+  </si>
+  <si>
+    <t>Beneficio</t>
+  </si>
+  <si>
+    <t>Beneficio Neto</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
+    <t>Gastos iniciales</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Gastos Anuales (se cargan a principio de año)</t>
+  </si>
+  <si>
+    <t>Gastos por horas (suponiendo que durante los 2 primeros meses se piden 20h, el tercer mes 10h y el resto de meses se hace un promedio de 5h al mes)</t>
+  </si>
+  <si>
+    <t>Gastos Mensuales</t>
+  </si>
+  <si>
+    <t>Beneficios mensuales</t>
+  </si>
+  <si>
+    <t>Beneficios mensuales y alumno (suponiendo que hay 6 clases y cada clase tiene 10 alumnos)</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>1º Mes</t>
+  </si>
+  <si>
+    <t>2º Mes</t>
+  </si>
+  <si>
+    <t>3º Mes</t>
+  </si>
+  <si>
+    <t>Resto de meses</t>
+  </si>
+  <si>
+    <t>Resto de mese</t>
+  </si>
+  <si>
+    <t>Gastos por hora y alumno (suponiendo que hay 8 empleados y que se da un curso intensivo de 8 horas durante 3 dias)</t>
   </si>
 </sst>
 </file>
@@ -342,7 +437,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,8 +462,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -391,11 +498,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -411,6 +568,31 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3057,7 +3239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
     </sheetView>
@@ -5386,4 +5568,2555 @@
   <autoFilter ref="A1:J1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="E1" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <f>20*F3</f>
+        <v>200</v>
+      </c>
+      <c r="H3" s="1">
+        <f>20*F3</f>
+        <v>200</v>
+      </c>
+      <c r="I3" s="1">
+        <f>10*F3</f>
+        <v>100</v>
+      </c>
+      <c r="J3" s="1">
+        <f>5*F3</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>60</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>200</v>
+      </c>
+      <c r="E7" s="1">
+        <v>16</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1">
+        <f>(8*(8*3))*F7</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>10</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>30000</v>
+      </c>
+      <c r="G14" s="1">
+        <v>5</v>
+      </c>
+      <c r="H14" s="1">
+        <v>50</v>
+      </c>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="G16" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>13</v>
+      </c>
+      <c r="C18" s="1">
+        <v>40</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <v>25</v>
+      </c>
+      <c r="I18" s="1">
+        <f>(6*10)*H18</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>25</v>
+      </c>
+      <c r="I19" s="1">
+        <f>(6*10)*H19</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="16"/>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="R25" s="10"/>
+      <c r="S25" s="10"/>
+      <c r="T25" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="U25" s="10"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="X25" s="10"/>
+      <c r="Y25" s="10"/>
+      <c r="Z25" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA25" s="10"/>
+      <c r="AB25" s="10"/>
+      <c r="AC25" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD25" s="10"/>
+      <c r="AE25" s="10"/>
+      <c r="AF25" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG25" s="10"/>
+      <c r="AH25" s="10"/>
+      <c r="AI25" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ25" s="10"/>
+      <c r="AK25" s="10"/>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="N26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="O26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="T26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="U26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="W26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="X26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH26" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI26" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ26" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK26" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1">
+        <f>500+100+60+25+200+70+60+10+0+0+1000+30000+40+200+3000+1920</f>
+        <v>37185</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <f>C27-B27</f>
+        <v>-37185</v>
+      </c>
+      <c r="E27" s="1">
+        <f>200+40</f>
+        <v>240</v>
+      </c>
+      <c r="F27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="G27" s="1">
+        <f>D27-E27+F27</f>
+        <v>-34275</v>
+      </c>
+      <c r="H27" s="1">
+        <f>100+40</f>
+        <v>140</v>
+      </c>
+      <c r="I27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="J27" s="1">
+        <f>G27-H27+I27</f>
+        <v>-31265</v>
+      </c>
+      <c r="K27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="M27" s="1">
+        <f>J27-K27+L27</f>
+        <v>-28205</v>
+      </c>
+      <c r="N27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="P27" s="1">
+        <f>M27-N27+O27</f>
+        <v>-25145</v>
+      </c>
+      <c r="Q27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="S27" s="1">
+        <f>P27-Q27+R27</f>
+        <v>-22085</v>
+      </c>
+      <c r="T27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="V27" s="1">
+        <f>S27-T27+U27</f>
+        <v>-19025</v>
+      </c>
+      <c r="W27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="Y27" s="1">
+        <f>V27-W27+X27</f>
+        <v>-15965</v>
+      </c>
+      <c r="Z27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AB27" s="1">
+        <f>Y27-Z27+AA27</f>
+        <v>-12905</v>
+      </c>
+      <c r="AC27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AE27" s="1">
+        <f>AB27-AC27+AD27</f>
+        <v>-9845</v>
+      </c>
+      <c r="AF27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AH27" s="1">
+        <f>AE27-AF27+AG27</f>
+        <v>-6785</v>
+      </c>
+      <c r="AI27" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ27" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AK27" s="1">
+        <f>AH27-AI27+AJ27</f>
+        <v>-3725</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>1</v>
+      </c>
+      <c r="B28" s="1">
+        <f>3000+50+40</f>
+        <v>3090</v>
+      </c>
+      <c r="C28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="D28" s="1">
+        <f>AK27-B28+C28</f>
+        <v>-3665</v>
+      </c>
+      <c r="E28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="F28" s="1">
+        <f t="shared" ref="F28:F31" si="0">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="G28" s="1">
+        <f t="shared" ref="G28:G29" si="1">D28-E28+F28</f>
+        <v>-605</v>
+      </c>
+      <c r="H28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" ref="I28:I31" si="2">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="J28" s="19">
+        <f t="shared" ref="J28:J29" si="3">G28-H28+I28</f>
+        <v>2455</v>
+      </c>
+      <c r="K28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L28" s="1">
+        <f t="shared" ref="L28:L31" si="4">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="M28" s="1">
+        <f t="shared" ref="M28:M29" si="5">J28-K28+L28</f>
+        <v>5515</v>
+      </c>
+      <c r="N28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O28" s="1">
+        <f t="shared" ref="O28:O31" si="6">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="P28" s="1">
+        <f t="shared" ref="P28:P29" si="7">M28-N28+O28</f>
+        <v>8575</v>
+      </c>
+      <c r="Q28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R28" s="1">
+        <f t="shared" ref="R28:R31" si="8">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="S28" s="1">
+        <f t="shared" ref="S28:S29" si="9">P28-Q28+R28</f>
+        <v>11635</v>
+      </c>
+      <c r="T28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U28" s="1">
+        <f t="shared" ref="U28:U31" si="10">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="V28" s="1">
+        <f t="shared" ref="V28:V29" si="11">S28-T28+U28</f>
+        <v>14695</v>
+      </c>
+      <c r="W28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X28" s="1">
+        <f t="shared" ref="X28:X31" si="12">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="Y28" s="1">
+        <f t="shared" ref="Y28:Y29" si="13">V28-W28+X28</f>
+        <v>17755</v>
+      </c>
+      <c r="Z28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA28" s="1">
+        <f t="shared" ref="AA28:AA31" si="14">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AB28" s="1">
+        <f t="shared" ref="AB28:AB29" si="15">Y28-Z28+AA28</f>
+        <v>20815</v>
+      </c>
+      <c r="AC28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD28" s="1">
+        <f t="shared" ref="AD28:AD31" si="16">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AE28" s="1">
+        <f t="shared" ref="AE28:AE29" si="17">AB28-AC28+AD28</f>
+        <v>23875</v>
+      </c>
+      <c r="AF28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG28" s="1">
+        <f t="shared" ref="AG28:AG31" si="18">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AH28" s="1">
+        <f t="shared" ref="AH28:AH29" si="19">AE28-AF28+AG28</f>
+        <v>26935</v>
+      </c>
+      <c r="AI28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ28" s="1">
+        <f t="shared" ref="AJ28:AJ31" si="20">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AK28" s="1">
+        <f t="shared" ref="AK28:AK29" si="21">AH28-AI28+AJ28</f>
+        <v>29995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>2</v>
+      </c>
+      <c r="B29" s="1">
+        <f>3000+50+40</f>
+        <v>3090</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" ref="C29:C31" si="22">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="D29" s="1">
+        <f>AK28-B29+C29</f>
+        <v>30055</v>
+      </c>
+      <c r="E29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" si="1"/>
+        <v>33115</v>
+      </c>
+      <c r="H29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="3"/>
+        <v>36175</v>
+      </c>
+      <c r="K29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" si="4"/>
+        <v>3150</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" si="5"/>
+        <v>39235</v>
+      </c>
+      <c r="N29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" si="6"/>
+        <v>3150</v>
+      </c>
+      <c r="P29" s="1">
+        <f t="shared" si="7"/>
+        <v>42295</v>
+      </c>
+      <c r="Q29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R29" s="1">
+        <f t="shared" si="8"/>
+        <v>3150</v>
+      </c>
+      <c r="S29" s="1">
+        <f t="shared" si="9"/>
+        <v>45355</v>
+      </c>
+      <c r="T29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U29" s="1">
+        <f t="shared" si="10"/>
+        <v>3150</v>
+      </c>
+      <c r="V29" s="1">
+        <f t="shared" si="11"/>
+        <v>48415</v>
+      </c>
+      <c r="W29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X29" s="1">
+        <f t="shared" si="12"/>
+        <v>3150</v>
+      </c>
+      <c r="Y29" s="1">
+        <f t="shared" si="13"/>
+        <v>51475</v>
+      </c>
+      <c r="Z29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA29" s="1">
+        <f t="shared" si="14"/>
+        <v>3150</v>
+      </c>
+      <c r="AB29" s="1">
+        <f t="shared" si="15"/>
+        <v>54535</v>
+      </c>
+      <c r="AC29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD29" s="1">
+        <f t="shared" si="16"/>
+        <v>3150</v>
+      </c>
+      <c r="AE29" s="1">
+        <f t="shared" si="17"/>
+        <v>57595</v>
+      </c>
+      <c r="AF29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG29" s="1">
+        <f t="shared" si="18"/>
+        <v>3150</v>
+      </c>
+      <c r="AH29" s="1">
+        <f t="shared" si="19"/>
+        <v>60655</v>
+      </c>
+      <c r="AI29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ29" s="1">
+        <f t="shared" si="20"/>
+        <v>3150</v>
+      </c>
+      <c r="AK29" s="1">
+        <f t="shared" si="21"/>
+        <v>63715</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>3</v>
+      </c>
+      <c r="B30" s="1">
+        <f>3000+50+40</f>
+        <v>3090</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="22"/>
+        <v>3150</v>
+      </c>
+      <c r="D30" s="1">
+        <f>AK29-B30+C30</f>
+        <v>63775</v>
+      </c>
+      <c r="E30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" ref="G30" si="23">D30-E30+F30</f>
+        <v>66835</v>
+      </c>
+      <c r="H30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" ref="J30" si="24">G30-H30+I30</f>
+        <v>69895</v>
+      </c>
+      <c r="K30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="4"/>
+        <v>3150</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" ref="M30" si="25">J30-K30+L30</f>
+        <v>72955</v>
+      </c>
+      <c r="N30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="6"/>
+        <v>3150</v>
+      </c>
+      <c r="P30" s="1">
+        <f t="shared" ref="P30" si="26">M30-N30+O30</f>
+        <v>76015</v>
+      </c>
+      <c r="Q30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" si="8"/>
+        <v>3150</v>
+      </c>
+      <c r="S30" s="1">
+        <f t="shared" ref="S30" si="27">P30-Q30+R30</f>
+        <v>79075</v>
+      </c>
+      <c r="T30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U30" s="1">
+        <f t="shared" si="10"/>
+        <v>3150</v>
+      </c>
+      <c r="V30" s="1">
+        <f t="shared" ref="V30" si="28">S30-T30+U30</f>
+        <v>82135</v>
+      </c>
+      <c r="W30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X30" s="1">
+        <f t="shared" si="12"/>
+        <v>3150</v>
+      </c>
+      <c r="Y30" s="1">
+        <f t="shared" ref="Y30" si="29">V30-W30+X30</f>
+        <v>85195</v>
+      </c>
+      <c r="Z30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA30" s="1">
+        <f t="shared" si="14"/>
+        <v>3150</v>
+      </c>
+      <c r="AB30" s="1">
+        <f t="shared" ref="AB30" si="30">Y30-Z30+AA30</f>
+        <v>88255</v>
+      </c>
+      <c r="AC30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD30" s="1">
+        <f t="shared" si="16"/>
+        <v>3150</v>
+      </c>
+      <c r="AE30" s="1">
+        <f t="shared" ref="AE30" si="31">AB30-AC30+AD30</f>
+        <v>91315</v>
+      </c>
+      <c r="AF30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG30" s="1">
+        <f t="shared" si="18"/>
+        <v>3150</v>
+      </c>
+      <c r="AH30" s="1">
+        <f t="shared" ref="AH30" si="32">AE30-AF30+AG30</f>
+        <v>94375</v>
+      </c>
+      <c r="AI30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ30" s="1">
+        <f t="shared" si="20"/>
+        <v>3150</v>
+      </c>
+      <c r="AK30" s="1">
+        <f t="shared" ref="AK30" si="33">AH30-AI30+AJ30</f>
+        <v>97435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1">
+        <f>3000+50+40</f>
+        <v>3090</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="22"/>
+        <v>3150</v>
+      </c>
+      <c r="D31" s="1">
+        <f>AK30-B31+C31</f>
+        <v>97495</v>
+      </c>
+      <c r="E31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" ref="G31" si="34">D31-E31+F31</f>
+        <v>100555</v>
+      </c>
+      <c r="H31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" ref="J31" si="35">G31-H31+I31</f>
+        <v>103615</v>
+      </c>
+      <c r="K31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="4"/>
+        <v>3150</v>
+      </c>
+      <c r="M31" s="6">
+        <f t="shared" ref="M31" si="36">J31-K31+L31</f>
+        <v>106675</v>
+      </c>
+      <c r="N31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O31" s="1">
+        <f t="shared" si="6"/>
+        <v>3150</v>
+      </c>
+      <c r="P31" s="1">
+        <f t="shared" ref="P31" si="37">M31-N31+O31</f>
+        <v>109735</v>
+      </c>
+      <c r="Q31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R31" s="1">
+        <f t="shared" si="8"/>
+        <v>3150</v>
+      </c>
+      <c r="S31" s="1">
+        <f t="shared" ref="S31" si="38">P31-Q31+R31</f>
+        <v>112795</v>
+      </c>
+      <c r="T31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U31" s="1">
+        <f t="shared" si="10"/>
+        <v>3150</v>
+      </c>
+      <c r="V31" s="1">
+        <f t="shared" ref="V31" si="39">S31-T31+U31</f>
+        <v>115855</v>
+      </c>
+      <c r="W31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X31" s="1">
+        <f t="shared" si="12"/>
+        <v>3150</v>
+      </c>
+      <c r="Y31" s="1">
+        <f t="shared" ref="Y31" si="40">V31-W31+X31</f>
+        <v>118915</v>
+      </c>
+      <c r="Z31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA31" s="1">
+        <f t="shared" si="14"/>
+        <v>3150</v>
+      </c>
+      <c r="AB31" s="1">
+        <f t="shared" ref="AB31" si="41">Y31-Z31+AA31</f>
+        <v>121975</v>
+      </c>
+      <c r="AC31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD31" s="1">
+        <f t="shared" si="16"/>
+        <v>3150</v>
+      </c>
+      <c r="AE31" s="1">
+        <f t="shared" ref="AE31" si="42">AB31-AC31+AD31</f>
+        <v>125035</v>
+      </c>
+      <c r="AF31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG31" s="1">
+        <f t="shared" si="18"/>
+        <v>3150</v>
+      </c>
+      <c r="AH31" s="1">
+        <f t="shared" ref="AH31" si="43">AE31-AF31+AG31</f>
+        <v>128095</v>
+      </c>
+      <c r="AI31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ31" s="1">
+        <f t="shared" si="20"/>
+        <v>3150</v>
+      </c>
+      <c r="AK31" s="1">
+        <f t="shared" ref="AK31" si="44">AH31-AI31+AJ31</f>
+        <v>131155</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="AI25:AK25"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="H25:J25"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="N25:P25"/>
+    <mergeCell ref="Q25:S25"/>
+    <mergeCell ref="T25:V25"/>
+    <mergeCell ref="W25:Y25"/>
+    <mergeCell ref="Z25:AB25"/>
+    <mergeCell ref="AC25:AE25"/>
+    <mergeCell ref="AF25:AH25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="E1" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>500</v>
+      </c>
+      <c r="E3" s="1">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1">
+        <f>20*F3</f>
+        <v>200</v>
+      </c>
+      <c r="H3" s="1">
+        <f>20*F3</f>
+        <v>200</v>
+      </c>
+      <c r="I3" s="1">
+        <f>10*F3</f>
+        <v>100</v>
+      </c>
+      <c r="J3" s="1">
+        <f>5*F3</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>60</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
+      <c r="G7" s="1">
+        <f>(8*(8*3))*F7</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2000</v>
+      </c>
+      <c r="G14" s="1">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <v>40000</v>
+      </c>
+      <c r="G15" s="1">
+        <v>5</v>
+      </c>
+      <c r="H15" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="G17" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1">
+        <v>40</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>25</v>
+      </c>
+      <c r="I19" s="1">
+        <f>(6*10)*H19</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <v>25</v>
+      </c>
+      <c r="I20" s="1">
+        <f>(6*10)*H20</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" s="16"/>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>13</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="O26" s="10"/>
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="R26" s="10"/>
+      <c r="S26" s="10"/>
+      <c r="T26" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="U26" s="10"/>
+      <c r="V26" s="10"/>
+      <c r="W26" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="X26" s="10"/>
+      <c r="Y26" s="10"/>
+      <c r="Z26" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA26" s="10"/>
+      <c r="AB26" s="10"/>
+      <c r="AC26" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="AD26" s="10"/>
+      <c r="AE26" s="10"/>
+      <c r="AF26" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG26" s="10"/>
+      <c r="AH26" s="10"/>
+      <c r="AI26" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ26" s="10"/>
+      <c r="AK26" s="10"/>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="N27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="O27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="R27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="S27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="T27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="U27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="V27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="W27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="X27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AA27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AC27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AE27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH27" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI27" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ27" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK27" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>0</v>
+      </c>
+      <c r="B28" s="1">
+        <f>500+230+100+60+25+200+70+60+10+0+0+2000+40000+40+3000+200+1920</f>
+        <v>48415</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <f>C28-B28</f>
+        <v>-48415</v>
+      </c>
+      <c r="E28" s="1">
+        <f>200+40</f>
+        <v>240</v>
+      </c>
+      <c r="F28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="G28" s="1">
+        <f>D28-E28+F28</f>
+        <v>-45505</v>
+      </c>
+      <c r="H28" s="1">
+        <f>100+40</f>
+        <v>140</v>
+      </c>
+      <c r="I28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="J28" s="1">
+        <f>G28-H28+I28</f>
+        <v>-42495</v>
+      </c>
+      <c r="K28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="M28" s="1">
+        <f>J28-K28+L28</f>
+        <v>-39435</v>
+      </c>
+      <c r="N28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="P28" s="1">
+        <f>M28-N28+O28</f>
+        <v>-36375</v>
+      </c>
+      <c r="Q28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="S28" s="1">
+        <f>P28-Q28+R28</f>
+        <v>-33315</v>
+      </c>
+      <c r="T28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="V28" s="1">
+        <f>S28-T28+U28</f>
+        <v>-30255</v>
+      </c>
+      <c r="W28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="Y28" s="1">
+        <f>V28-W28+X28</f>
+        <v>-27195</v>
+      </c>
+      <c r="Z28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AB28" s="1">
+        <f>Y28-Z28+AA28</f>
+        <v>-24135</v>
+      </c>
+      <c r="AC28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AE28" s="1">
+        <f>AB28-AC28+AD28</f>
+        <v>-21075</v>
+      </c>
+      <c r="AF28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AH28" s="1">
+        <f>AE28-AF28+AG28</f>
+        <v>-18015</v>
+      </c>
+      <c r="AI28" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ28" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AK28" s="1">
+        <f>AH28-AI28+AJ28</f>
+        <v>-14955</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1</v>
+      </c>
+      <c r="B29" s="1">
+        <f>3000+50+40</f>
+        <v>3090</v>
+      </c>
+      <c r="C29" s="1">
+        <f>50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="D29" s="1">
+        <f>AK28-B29+C29</f>
+        <v>-14895</v>
+      </c>
+      <c r="E29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="F29" s="1">
+        <f t="shared" ref="F29:F32" si="0">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="G29" s="1">
+        <f t="shared" ref="G29:G32" si="1">D29-E29+F29</f>
+        <v>-11835</v>
+      </c>
+      <c r="H29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" ref="I29:I32" si="2">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" ref="J29:J32" si="3">G29-H29+I29</f>
+        <v>-8775</v>
+      </c>
+      <c r="K29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L29" s="1">
+        <f t="shared" ref="L29:L32" si="4">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="M29" s="1">
+        <f t="shared" ref="M29:M32" si="5">J29-K29+L29</f>
+        <v>-5715</v>
+      </c>
+      <c r="N29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O29" s="1">
+        <f t="shared" ref="O29:O32" si="6">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="P29" s="1">
+        <f t="shared" ref="P29:P32" si="7">M29-N29+O29</f>
+        <v>-2655</v>
+      </c>
+      <c r="Q29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R29" s="1">
+        <f t="shared" ref="R29:R32" si="8">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="S29" s="19">
+        <f t="shared" ref="S29:S32" si="9">P29-Q29+R29</f>
+        <v>405</v>
+      </c>
+      <c r="T29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U29" s="1">
+        <f t="shared" ref="U29:U32" si="10">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="V29" s="1">
+        <f t="shared" ref="V29:V32" si="11">S29-T29+U29</f>
+        <v>3465</v>
+      </c>
+      <c r="W29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X29" s="1">
+        <f t="shared" ref="X29:X32" si="12">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="Y29" s="1">
+        <f t="shared" ref="Y29:Y32" si="13">V29-W29+X29</f>
+        <v>6525</v>
+      </c>
+      <c r="Z29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA29" s="1">
+        <f t="shared" ref="AA29:AA32" si="14">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AB29" s="1">
+        <f t="shared" ref="AB29:AB32" si="15">Y29-Z29+AA29</f>
+        <v>9585</v>
+      </c>
+      <c r="AC29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD29" s="1">
+        <f t="shared" ref="AD29:AD32" si="16">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AE29" s="1">
+        <f t="shared" ref="AE29:AE32" si="17">AB29-AC29+AD29</f>
+        <v>12645</v>
+      </c>
+      <c r="AF29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG29" s="1">
+        <f t="shared" ref="AG29:AG32" si="18">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AH29" s="1">
+        <f t="shared" ref="AH29:AH32" si="19">AE29-AF29+AG29</f>
+        <v>15705</v>
+      </c>
+      <c r="AI29" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ29" s="1">
+        <f t="shared" ref="AJ29:AJ32" si="20">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="AK29" s="1">
+        <f t="shared" ref="AK29:AK32" si="21">AH29-AI29+AJ29</f>
+        <v>18765</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1">
+        <f t="shared" ref="B30:B32" si="22">3000+50+40</f>
+        <v>3090</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" ref="C30:C32" si="23">50+50+50+1500+1500</f>
+        <v>3150</v>
+      </c>
+      <c r="D30" s="1">
+        <f>AK29-B30+C30</f>
+        <v>18825</v>
+      </c>
+      <c r="E30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="F30" s="1">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="G30" s="1">
+        <f t="shared" si="1"/>
+        <v>21885</v>
+      </c>
+      <c r="H30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="3"/>
+        <v>24945</v>
+      </c>
+      <c r="K30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L30" s="1">
+        <f t="shared" si="4"/>
+        <v>3150</v>
+      </c>
+      <c r="M30" s="1">
+        <f t="shared" si="5"/>
+        <v>28005</v>
+      </c>
+      <c r="N30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O30" s="1">
+        <f t="shared" si="6"/>
+        <v>3150</v>
+      </c>
+      <c r="P30" s="1">
+        <f t="shared" si="7"/>
+        <v>31065</v>
+      </c>
+      <c r="Q30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R30" s="1">
+        <f t="shared" si="8"/>
+        <v>3150</v>
+      </c>
+      <c r="S30" s="1">
+        <f t="shared" si="9"/>
+        <v>34125</v>
+      </c>
+      <c r="T30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U30" s="1">
+        <f t="shared" si="10"/>
+        <v>3150</v>
+      </c>
+      <c r="V30" s="1">
+        <f t="shared" si="11"/>
+        <v>37185</v>
+      </c>
+      <c r="W30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X30" s="1">
+        <f t="shared" si="12"/>
+        <v>3150</v>
+      </c>
+      <c r="Y30" s="1">
+        <f t="shared" si="13"/>
+        <v>40245</v>
+      </c>
+      <c r="Z30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA30" s="1">
+        <f t="shared" si="14"/>
+        <v>3150</v>
+      </c>
+      <c r="AB30" s="1">
+        <f t="shared" si="15"/>
+        <v>43305</v>
+      </c>
+      <c r="AC30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD30" s="1">
+        <f t="shared" si="16"/>
+        <v>3150</v>
+      </c>
+      <c r="AE30" s="1">
+        <f t="shared" si="17"/>
+        <v>46365</v>
+      </c>
+      <c r="AF30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG30" s="1">
+        <f t="shared" si="18"/>
+        <v>3150</v>
+      </c>
+      <c r="AH30" s="1">
+        <f t="shared" si="19"/>
+        <v>49425</v>
+      </c>
+      <c r="AI30" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ30" s="1">
+        <f t="shared" si="20"/>
+        <v>3150</v>
+      </c>
+      <c r="AK30" s="1">
+        <f t="shared" si="21"/>
+        <v>52485</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>3</v>
+      </c>
+      <c r="B31" s="1">
+        <f t="shared" si="22"/>
+        <v>3090</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="23"/>
+        <v>3150</v>
+      </c>
+      <c r="D31" s="1">
+        <f>AK30-B31+C31</f>
+        <v>52545</v>
+      </c>
+      <c r="E31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="F31" s="1">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="G31" s="1">
+        <f t="shared" si="1"/>
+        <v>55605</v>
+      </c>
+      <c r="H31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="3"/>
+        <v>58665</v>
+      </c>
+      <c r="K31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="4"/>
+        <v>3150</v>
+      </c>
+      <c r="M31" s="1">
+        <f t="shared" si="5"/>
+        <v>61725</v>
+      </c>
+      <c r="N31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O31" s="1">
+        <f t="shared" si="6"/>
+        <v>3150</v>
+      </c>
+      <c r="P31" s="1">
+        <f t="shared" si="7"/>
+        <v>64785</v>
+      </c>
+      <c r="Q31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R31" s="1">
+        <f t="shared" si="8"/>
+        <v>3150</v>
+      </c>
+      <c r="S31" s="1">
+        <f t="shared" si="9"/>
+        <v>67845</v>
+      </c>
+      <c r="T31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U31" s="1">
+        <f t="shared" si="10"/>
+        <v>3150</v>
+      </c>
+      <c r="V31" s="1">
+        <f t="shared" si="11"/>
+        <v>70905</v>
+      </c>
+      <c r="W31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X31" s="1">
+        <f t="shared" si="12"/>
+        <v>3150</v>
+      </c>
+      <c r="Y31" s="1">
+        <f t="shared" si="13"/>
+        <v>73965</v>
+      </c>
+      <c r="Z31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA31" s="1">
+        <f t="shared" si="14"/>
+        <v>3150</v>
+      </c>
+      <c r="AB31" s="1">
+        <f t="shared" si="15"/>
+        <v>77025</v>
+      </c>
+      <c r="AC31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD31" s="1">
+        <f t="shared" si="16"/>
+        <v>3150</v>
+      </c>
+      <c r="AE31" s="1">
+        <f t="shared" si="17"/>
+        <v>80085</v>
+      </c>
+      <c r="AF31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG31" s="1">
+        <f t="shared" si="18"/>
+        <v>3150</v>
+      </c>
+      <c r="AH31" s="1">
+        <f t="shared" si="19"/>
+        <v>83145</v>
+      </c>
+      <c r="AI31" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ31" s="1">
+        <f t="shared" si="20"/>
+        <v>3150</v>
+      </c>
+      <c r="AK31" s="1">
+        <f t="shared" si="21"/>
+        <v>86205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1">
+        <f t="shared" si="22"/>
+        <v>3090</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="23"/>
+        <v>3150</v>
+      </c>
+      <c r="D32" s="1">
+        <f>AK31-B32+C32</f>
+        <v>86265</v>
+      </c>
+      <c r="E32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="F32" s="1">
+        <f t="shared" si="0"/>
+        <v>3150</v>
+      </c>
+      <c r="G32" s="1">
+        <f t="shared" si="1"/>
+        <v>89325</v>
+      </c>
+      <c r="H32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="2"/>
+        <v>3150</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="3"/>
+        <v>92385</v>
+      </c>
+      <c r="K32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="L32" s="1">
+        <f t="shared" si="4"/>
+        <v>3150</v>
+      </c>
+      <c r="M32" s="6">
+        <f t="shared" si="5"/>
+        <v>95445</v>
+      </c>
+      <c r="N32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="O32" s="1">
+        <f t="shared" si="6"/>
+        <v>3150</v>
+      </c>
+      <c r="P32" s="1">
+        <f t="shared" si="7"/>
+        <v>98505</v>
+      </c>
+      <c r="Q32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="R32" s="1">
+        <f t="shared" si="8"/>
+        <v>3150</v>
+      </c>
+      <c r="S32" s="1">
+        <f t="shared" si="9"/>
+        <v>101565</v>
+      </c>
+      <c r="T32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="U32" s="1">
+        <f t="shared" si="10"/>
+        <v>3150</v>
+      </c>
+      <c r="V32" s="1">
+        <f t="shared" si="11"/>
+        <v>104625</v>
+      </c>
+      <c r="W32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="X32" s="1">
+        <f t="shared" si="12"/>
+        <v>3150</v>
+      </c>
+      <c r="Y32" s="1">
+        <f t="shared" si="13"/>
+        <v>107685</v>
+      </c>
+      <c r="Z32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AA32" s="1">
+        <f t="shared" si="14"/>
+        <v>3150</v>
+      </c>
+      <c r="AB32" s="1">
+        <f t="shared" si="15"/>
+        <v>110745</v>
+      </c>
+      <c r="AC32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AD32" s="1">
+        <f t="shared" si="16"/>
+        <v>3150</v>
+      </c>
+      <c r="AE32" s="1">
+        <f t="shared" si="17"/>
+        <v>113805</v>
+      </c>
+      <c r="AF32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AG32" s="1">
+        <f t="shared" si="18"/>
+        <v>3150</v>
+      </c>
+      <c r="AH32" s="1">
+        <f t="shared" si="19"/>
+        <v>116865</v>
+      </c>
+      <c r="AI32" s="1">
+        <f>50+40</f>
+        <v>90</v>
+      </c>
+      <c r="AJ32" s="1">
+        <f t="shared" si="20"/>
+        <v>3150</v>
+      </c>
+      <c r="AK32" s="1">
+        <f t="shared" si="21"/>
+        <v>119925</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="AF26:AH26"/>
+    <mergeCell ref="AI26:AK26"/>
+    <mergeCell ref="Q26:S26"/>
+    <mergeCell ref="T26:V26"/>
+    <mergeCell ref="W26:Y26"/>
+    <mergeCell ref="Z26:AB26"/>
+    <mergeCell ref="AC26:AE26"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:P26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>